<commit_message>
updates to validation files
</commit_message>
<xml_diff>
--- a/schemaExamples/Croissant-fields.xlsx
+++ b/schemaExamples/Croissant-fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/CDIF/validation/schemaExamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="8_{4ED8F3AB-B96C-42E0-A92F-E961771FA1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{872B094D-BA17-4743-BD14-AFCAFF670756}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{4ED8F3AB-B96C-42E0-A92F-E961771FA1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6E7646D-2598-42AB-B51E-891B2D071D7D}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="263" yWindow="240" windowWidth="18990" windowHeight="9495" xr2:uid="{27DFB776-2C83-4927-B43C-E2DD7A3850B8}"/>
+    <workbookView xWindow="10695" yWindow="3990" windowWidth="17250" windowHeight="9720" xr2:uid="{27DFB776-2C83-4927-B43C-E2DD7A3850B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,12 +649,6 @@
       <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -708,14 +702,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -740,28 +728,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -792,6 +763,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1151,1315 +1125,1313 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="9.19921875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.46484375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" customWidth="1"/>
-    <col min="8" max="8" width="6.265625" customWidth="1"/>
-    <col min="9" max="9" width="58.86328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="58.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="17">
         <v>1</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="21" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="17">
         <v>1</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="17">
         <v>1</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="23" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B15" s="29" t="s">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="17">
         <v>1</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B18" s="29" t="s">
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B19" s="29" t="s">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="23" t="s">
+    <row r="20" spans="1:9" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B21" s="29" t="s">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="57" x14ac:dyDescent="0.45">
-      <c r="B22" s="29" t="s">
+    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="15" t="s">
+      <c r="E22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="57" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20" t="s">
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="16">
         <v>1</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D26" s="9" t="s">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="H27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="I27" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D28" s="9" t="s">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A30" s="10"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="10" t="s">
+    <row r="30" spans="1:9" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="E30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="10" t="s">
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="C33" s="10" t="s">
+      <c r="C32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="C33" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20" t="s">
+      <c r="E33" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="C34" s="10" t="s">
+    <row r="34" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="E34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="57" x14ac:dyDescent="0.45">
-      <c r="C35" s="10" t="s">
+    <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="C35" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="15" t="s">
+      <c r="E35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="I35" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C36" s="10" t="s">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C36" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="15" t="s">
+      <c r="E36" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="100.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="10" t="s">
+    <row r="37" spans="1:9" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="20" t="s">
+      <c r="E37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B38" s="25"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="9" t="s">
+    <row r="38" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="16"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="15" t="s">
+      <c r="E38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="H38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="15" t="s">
+      <c r="I38" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="10" t="s">
+    <row r="39" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="9" t="s">
+      <c r="B39" s="16"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F39" s="15" t="s">
+      <c r="E39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="G39" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="15" t="s">
+      <c r="H39" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="15" t="s">
+      <c r="I39" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="57" x14ac:dyDescent="0.45">
-      <c r="C40" s="10" t="s">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="15" t="s">
+      <c r="E40" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="15" t="s">
+      <c r="I40" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="10"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="9" t="s">
+    <row r="41" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F41" s="15" t="s">
+      <c r="E41" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G41" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="19" t="s">
+      <c r="E42" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F43" s="10" t="s">
+      <c r="E43" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="H43" s="10" t="s">
+      <c r="H43" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I43" s="10" t="s">
+      <c r="I43" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="10" t="s">
+    <row r="44" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F44" s="10" t="s">
+      <c r="E44" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="10" t="s">
+      <c r="I44" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D45" s="10" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E45" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F45" s="10" t="s">
+      <c r="E45" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="H45" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="I45" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A46" s="10" t="s">
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F46" s="10" t="s">
+      <c r="E46" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H46" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I46" s="10" t="s">
+      <c r="I46" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="10" t="s">
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F47" s="10" t="s">
+      <c r="E47" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G47" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="H47" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="10" t="s">
+      <c r="I47" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D48" s="10" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D48" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="10" t="s">
+      <c r="E48" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="H48" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="10" t="s">
+      <c r="I48" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C49" s="10" t="s">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C49" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F49" s="10" t="s">
+      <c r="E49" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G49" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H49" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I49" s="10" t="s">
+      <c r="I49" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="C50" s="10" t="s">
+    <row r="50" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="C50" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E50" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20" t="s">
+      <c r="E50" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D51" s="10" t="s">
+    <row r="51" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E51" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F51" s="9" t="s">
+      <c r="E51" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="9" t="s">
+      <c r="H51" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D52" s="10" t="s">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D52" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E52" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F52" s="9" t="s">
+      <c r="E52" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F52" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H52" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I52" s="9" t="s">
+      <c r="I52" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D53" s="10" t="s">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D53" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E53" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F53" s="9" t="s">
+      <c r="E53" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="H53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I53" s="9" t="s">
+      <c r="I53" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D54" s="10" t="s">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D54" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E54" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F54" s="9" t="s">
+      <c r="E54" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G54" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H54" s="9" t="s">
+      <c r="H54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="I54" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D55" s="10" t="s">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D55" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E55" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F55" s="9" t="s">
+      <c r="E55" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G55" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H55" s="9" t="s">
+      <c r="H55" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I55" s="9" t="s">
+      <c r="I55" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A56" s="10" t="s">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E56" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="9" t="s">
+      <c r="E56" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="I56" s="7" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>